<commit_message>
without .env and mail in xlsx
</commit_message>
<xml_diff>
--- a/Precios amazon.xlsx
+++ b/Precios amazon.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1714,6 +1714,1042 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Coach Men's Coin Wallet</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>$85.36</t>
+        </is>
+      </c>
+      <c r="E46" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/COACH-Compact-Bifold-Wallet-74991/dp/B012U0BS2G/ref=sr_1_48?keywords=billetera&amp;qid=1658863694&amp;sr=8-48</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Fidelo Minimalist Wallets Card Wallet - Hybrid RFID Wallets for Men Slim Wallet</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>$24.99</t>
+        </is>
+      </c>
+      <c r="E47" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/FIDELO-Minimalist-Wallet-Men-Wallets/dp/B07F64QYY1/ref=sr_1_45?keywords=billetera&amp;qid=1658863694&amp;sr=8-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Champion Graphic Wallet</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>$14.19</t>
+        </is>
+      </c>
+      <c r="E48" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Champion-Rhyme-Bifold-Wallet-black/dp/B07NY1DHM9/ref=sr_1_42?keywords=billetera&amp;qid=1658863694&amp;sr=8-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Slim RFID Wallets for Men - Genuine Leather Front Pocket Trifold Wallet</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>$9.99</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/RFID-Leather-Trifold-Wallets-Men/dp/B0796PTVLR/ref=sr_1_24?keywords=billetera&amp;qid=1658863694&amp;sr=8-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Zitahli Wallet for Men Slim Larger Capacity with 12 Slots RFID Blocking Men's Wallet Minimalist Front Pocket Bifold Leather with ID Window Gift Box</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>$22.95</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Zitahli-Wallets-Bifold-Leather-Minimalist/dp/B09MLRW8GP/ref=sr_1_27?keywords=billetera&amp;qid=1658863694&amp;sr=8-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>TRAVANDO Mens Slim Wallet with Money Clip AUSTIN RFID Blocking Bifold Credit Card Holder for Men with Gift Box</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>$23.74</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/TRAVANDO-Wallet-AUSTIN-Blocking-Bifold/dp/B09V19STJZ/ref=sr_1_26?keywords=billetera&amp;qid=1658863694&amp;sr=8-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>TRAVANDO Mens Slim Wallet with Money Clip AUSTIN RFID Blocking Bifold Credit Card Holder for Men with Gift Box</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>$23.74</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A01646681XFS2GZH69N92&amp;url=%2FTRAVANDO-Wallet-Blocking-Credit-Minimalist%2Fdp%2FB07FPVR858%2Fref%3Dsr_1_1_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863694%26sr%3D8-1-spons%26psc%3D1&amp;qualifier=1658863694&amp;id=2238914241692446&amp;widgetName=sp_atf</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Steve Madden Men's Leather RFID Wallet Extra Capacity Attached Flip Pocket</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>$10.71</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Steve-Madden-Leather-Capacity-Attached/dp/B074CHD9C8/ref=sr_1_omk_6?keywords=billetera&amp;qid=1658863694&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Columbia Men's RFID Trifold Wallet</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>$22.00</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Columbia-Blocking-Trifold-Security-Newberry/dp/B00GBC693I/ref=sr_1_15?keywords=billetera&amp;qid=1658863694&amp;sr=8-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Buffway Slim Minimalist Front Pocket RFID Blocking Leather Wallets for Men Women</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>$14.99</t>
+        </is>
+      </c>
+      <c r="E55" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Slim-Minimalist-Leather-Wallets-Women/dp/B07SVPD6PX/ref=sr_1_51?keywords=billetera&amp;qid=1658863694&amp;sr=8-51</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Front Pocket Wallet for Men - RFID Blocking Leather Bifold Wallet with ID Window (Coal)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>$12.99</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Slim-RFID-Bifold-Wallets-Men/dp/B07M8L5823/ref=sr_1_12?keywords=billetera&amp;qid=1658863694&amp;sr=8-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Mountain Voyage Slim Minimalist RFID Blocking Men Wallet - Men Black Metal Credit Card Holder with Money Clip - Wallet Mens Slim - Wallets Mens Easily Removable Money &amp; Card - Wallets Men Metal</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>$39.99</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A00514821L1JT6ZY91OS7&amp;url=%2FMountain-Voyage-Minimalist-Blocking-Wallet%2Fdp%2FB09TRTHLGX%2Fref%3Dsr_1_4_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863694%26sr%3D8-4-spons%26psc%3D1&amp;qualifier=1658863694&amp;id=2238914241692446&amp;widgetName=sp_atf</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Timberland Men's Genuine Leather RFID Blocking Trifold Wallet</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>$15.94</t>
+        </is>
+      </c>
+      <c r="E58" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Timberland-Genuine-Leather-Blocking-Security/dp/B01MCULY6Y/ref=sr_1_8?keywords=billetera&amp;qid=1658863694&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Columbia Men's RFID Passcase Wallet</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>$25.60</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Columbia-Blocking-Passcase-Wallet-Deschutes/dp/B07K2NZM6G/ref=sr_1_19?keywords=billetera&amp;qid=1658863694&amp;sr=8-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="5" t="n">
+        <v>44768.60297101852</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Furid 30/0FF Money Clip, Slim Metal Wallet, Minimalist Wallet For Men, Credit Card Holder Wallets for Men Gift(Green), Tactical Wallet</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>$21.99</t>
+        </is>
+      </c>
+      <c r="E60" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_btf_aps_sr_pg1_1?ie=UTF8&amp;adId=A09748672SOSAVXR97FGW&amp;url=%2FWallet-Minimalist-Credit-Holder-Wallets%2Fdp%2FB09BNT1TRK%2Fref%3Dsr_1_57_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863694%26sr%3D8-57-spons%26psc%3D1&amp;qualifier=1658863694&amp;id=2238914241692446&amp;widgetName=sp_btf</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Timberland Men's Leather Wallet with Attached Flip Pocket</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>$17.28</t>
+        </is>
+      </c>
+      <c r="E61" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Timberland-Leather-Wallet-Attached-Pocket/dp/B00FJ1TTXO/ref=sr_1_18?keywords=billetera&amp;qid=1658863694&amp;sr=8-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="5" t="n">
+        <v>44768.60297084491</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>SERMAN BRANDS Money Clip Wallet - Mens Wallets slim Front Pocket RFID Blocking Card Holder Minimalist Mini Bifold</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>$29.95</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/SERMAN-BRANDS-Money-Clip-Wallet/dp/B084CVTW8J/ref=sr_1_44?keywords=billetera&amp;qid=1658863694&amp;sr=8-44</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="5" t="n">
+        <v>44768.60297065973</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>RUNBOX Slim Wallet for Men Minimalist Leather Bifold RFID Blocking with Gift Box</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>$25.99</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Runbox-Leather-Wallets-Blocking-Capacity/dp/B092VR48NK/ref=sr_1_14?keywords=billetera&amp;qid=1658863694&amp;sr=8-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Coach Men's Coin Wallet</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>$85.36</t>
+        </is>
+      </c>
+      <c r="E64" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/COACH-Compact-Bifold-Wallet-74991/dp/B012U0BS2G/ref=sr_1_49?keywords=billetera&amp;qid=1658863721&amp;sr=8-49</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Fidelo Minimalist Wallets Card Wallet - Hybrid RFID Wallets for Men Slim Wallet</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>$24.99</t>
+        </is>
+      </c>
+      <c r="E65" s="4" t="n">
+        <v>51</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/FIDELO-Minimalist-Wallet-Men-Wallets/dp/B07F64QYY1/ref=sr_1_46?keywords=billetera&amp;qid=1658863721&amp;sr=8-46</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Zitahli Wallet for Men Slim Larger Capacity with 12 Slots RFID Blocking Men's Wallet Minimalist Front Pocket Bifold Leather with ID Window Gift Box</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>$22.95</t>
+        </is>
+      </c>
+      <c r="E66" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Zitahli-Wallets-Bifold-Leather-Minimalist/dp/B09MLRW8GP/ref=sr_1_28?keywords=billetera&amp;qid=1658863721&amp;sr=8-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>TRAVANDO Mens Slim Wallet with Money Clip AUSTIN RFID Blocking Bifold Credit Card Holder for Men with Gift Box</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>$23.74</t>
+        </is>
+      </c>
+      <c r="E67" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A01646681XFS2GZH69N92&amp;url=%2FTRAVANDO-Wallet-Blocking-Credit-Minimalist%2Fdp%2FB07FPVR858%2Fref%3Dsr_1_1_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863721%26sr%3D8-1-spons%26psc%3D1&amp;qualifier=1658863721&amp;id=3104504931987830&amp;widgetName=sp_atf</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>TRAVANDO Mens Slim Wallet with Money Clip AUSTIN RFID Blocking Bifold Credit Card Holder for Men with Gift Box</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>$23.74</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/TRAVANDO-Wallet-AUSTIN-Blocking-Bifold/dp/B09V19STJZ/ref=sr_1_27?keywords=billetera&amp;qid=1658863721&amp;sr=8-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Steve Madden Men's Leather RFID Wallet Extra Capacity Attached Flip Pocket</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>$10.71</t>
+        </is>
+      </c>
+      <c r="E69" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Steve-Madden-Leather-Capacity-Attached/dp/B074CHD9C8/ref=sr_1_6?keywords=billetera&amp;qid=1658863721&amp;sr=8-6</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Columbia Men's RFID Trifold Wallet</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>$22.00</t>
+        </is>
+      </c>
+      <c r="E70" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Columbia-Blocking-Trifold-Security-Newberry/dp/B00GBC693I/ref=sr_1_16?keywords=billetera&amp;qid=1658863721&amp;sr=8-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Timberland Women's Leather RFID Flap Wallet Clutch Organizer</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>$22.37</t>
+        </is>
+      </c>
+      <c r="E71" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Timberland-Leather-Wallet-Clutch-Organizer/dp/B07T2F1VFJ/ref=sr_1_42?keywords=billetera&amp;qid=1658863721&amp;sr=8-42</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Buffway Slim Minimalist Front Pocket RFID Blocking Leather Wallets for Men Women</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>$14.99</t>
+        </is>
+      </c>
+      <c r="E72" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Slim-Minimalist-Leather-Wallets-Women/dp/B07SVPD6PX/ref=sr_1_52?keywords=billetera&amp;qid=1658863721&amp;sr=8-52</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Front Pocket Wallet for Men - RFID Blocking Leather Bifold Wallet with ID Window (Coal)</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>$12.99</t>
+        </is>
+      </c>
+      <c r="E73" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Slim-RFID-Bifold-Wallets-Men/dp/B07M8L5823/ref=sr_1_12?keywords=billetera&amp;qid=1658863721&amp;sr=8-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Timberland Men's Genuine Leather RFID Blocking Trifold Wallet</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>$15.94</t>
+        </is>
+      </c>
+      <c r="E74" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Timberland-Genuine-Leather-Blocking-Security/dp/B01MCULY6Y/ref=sr_1_8?keywords=billetera&amp;qid=1658863721&amp;sr=8-8</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5" t="n">
+        <v>44768.60328368055</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Mens Wallet with Chain Genuine Leather Purse RFID Blocking Bifold Double Zipper Coin Pocket with Anti-Theft Chain</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>$23.99</t>
+        </is>
+      </c>
+      <c r="E75" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_btf_aps_sr_pg1_1?ie=UTF8&amp;adId=A03990732AJVWVIJZS1VD&amp;url=%2FWallet-Genuine-Leather-Blocking-Anti-Theft%2Fdp%2FB097LL1SR5%2Fref%3Dsr_1_59_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863721%26sr%3D8-59-spons%26psc%3D1%26smid%3DA1YHZ54GOJ30V7&amp;qualifier=1658863721&amp;id=3104504931987830&amp;widgetName=sp_btf</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Mountain Voyage Slim Minimalist RFID Blocking Men Wallet - Men Black Metal Credit Card Holder with Money Clip - Wallet Mens Slim - Wallets Mens Easily Removable Money &amp; Card - Wallets Men Metal</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>$39.99</t>
+        </is>
+      </c>
+      <c r="E76" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_aps_sr_pg1_1?ie=UTF8&amp;adId=A00514821L1JT6ZY91OS7&amp;url=%2FMountain-Voyage-Minimalist-Blocking-Wallet%2Fdp%2FB09TRTHLGX%2Fref%3Dsr_1_4_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863721%26sr%3D8-4-spons%26psc%3D1&amp;qualifier=1658863721&amp;id=3104504931987830&amp;widgetName=sp_atf</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Columbia Men's RFID Passcase Wallet</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>$25.60</t>
+        </is>
+      </c>
+      <c r="E77" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Columbia-Blocking-Passcase-Wallet-Deschutes/dp/B07K2NZM6G/ref=sr_1_20?keywords=billetera&amp;qid=1658863721&amp;sr=8-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="n">
+        <v>44768.60328368055</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Furid 30/0FF Money Clip, Slim Metal Wallet, Minimalist Wallet For Men, Credit Card Holder Wallets for Men Gift(Green), Tactical Wallet</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>$21.99</t>
+        </is>
+      </c>
+      <c r="E78" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/gp/slredirect/picassoRedirect.html/ref=pa_sp_btf_aps_sr_pg1_1?ie=UTF8&amp;adId=A09748672SOSAVXR97FGW&amp;url=%2FWallet-Minimalist-Credit-Holder-Wallets%2Fdp%2FB09BNT1TRK%2Fref%3Dsr_1_57_sspa%3Fkeywords%3Dbilletera%26qid%3D1658863721%26sr%3D8-57-spons%26psc%3D1&amp;qualifier=1658863721&amp;id=3104504931987830&amp;widgetName=sp_btf</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SERMAN BRANDS Money Clip Wallet - Mens Wallets slim Front Pocket RFID Blocking Card Holder Minimalist Mini Bifold</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>$29.95</t>
+        </is>
+      </c>
+      <c r="E79" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/SERMAN-BRANDS-Money-Clip-Wallet/dp/B084CVTW8J/ref=sr_1_45?keywords=billetera&amp;qid=1658863721&amp;sr=8-45</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5" t="n">
+        <v>44768.60328349537</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Timberland Men's Leather Wallet with Attached Flip Pocket</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>$17.28</t>
+        </is>
+      </c>
+      <c r="E80" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Timberland-Leather-Wallet-Attached-Pocket/dp/B00FJ1TTXO/ref=sr_1_19?keywords=billetera&amp;qid=1658863721&amp;sr=8-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>RUNBOX Slim Wallet for Men Minimalist Leather Bifold RFID Blocking with Gift Box</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>$25.99</t>
+        </is>
+      </c>
+      <c r="E81" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Runbox-Leather-Wallets-Blocking-Capacity/dp/B092VR48NK/ref=sr_1_15?keywords=billetera&amp;qid=1658863721&amp;sr=8-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5" t="n">
+        <v>44768.60328331019</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>billetera</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Nautica Women's Perfect Carry-All Money Manager Oraganizer with RFID Blocking Wallet</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>$18.85</t>
+        </is>
+      </c>
+      <c r="E82" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com/-/es/Nautica-Perfect-Carry-All-Oraganizer-Blocking/dp/B07G3LDMT6/ref=sr_1_14?keywords=billetera&amp;qid=1658863721&amp;sr=8-14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>